<commit_message>
create separate columns for system 4 and 6
</commit_message>
<xml_diff>
--- a/measures/btap_apply_necb_rules/regional_fuel_type_defaults.xlsx
+++ b/measures/btap_apply_necb_rules/regional_fuel_type_defaults.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="240" windowWidth="19440" windowHeight="11640"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="114">
   <si>
     <t>Province</t>
   </si>
@@ -351,17 +351,20 @@
     <t>fan_type</t>
   </si>
   <si>
-    <t>heating_coil_type_sys4and6</t>
-  </si>
-  <si>
     <t>var_speed_drive</t>
+  </si>
+  <si>
+    <t>heating_coil_type_sys4</t>
+  </si>
+  <si>
+    <t>heating_coil_type_sys6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,6 +511,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -542,6 +546,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -717,14 +722,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -735,12 +740,12 @@
     <col min="7" max="7" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="11" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1">
+    <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
@@ -769,13 +774,16 @@
         <v>94</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -806,11 +814,14 @@
       <c r="J2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="K2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -841,11 +852,14 @@
       <c r="J3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="K3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -876,11 +890,14 @@
       <c r="J4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="K4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -911,11 +928,14 @@
       <c r="J5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="K5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -946,11 +966,14 @@
       <c r="J6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="K6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -981,11 +1004,14 @@
       <c r="J7" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="K7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -1016,11 +1042,14 @@
       <c r="J8" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="K8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -1051,11 +1080,14 @@
       <c r="J9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="K9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -1086,11 +1118,14 @@
       <c r="J10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="K10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -1121,11 +1156,14 @@
       <c r="J11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="K11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -1156,12 +1194,14 @@
       <c r="J12" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L12" s="2"/>
+      <c r="K12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="2"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1170,8 +1210,9 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
@@ -1202,11 +1243,14 @@
       <c r="J13" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="K13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -1237,11 +1281,14 @@
       <c r="J14" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="K14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -1272,10 +1319,12 @@
       <c r="J15" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N15" s="3"/>
+      <c r="K15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -1284,8 +1333,9 @@
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15" s="3"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
@@ -1316,11 +1366,14 @@
       <c r="J16" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="K16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -1351,10 +1404,12 @@
       <c r="J17" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N17" s="3"/>
+      <c r="K17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -1363,8 +1418,9 @@
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17" s="3"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>77</v>
       </c>
@@ -1395,11 +1451,14 @@
       <c r="J18" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="K18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -1430,11 +1489,14 @@
       <c r="J19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="K19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>82</v>
       </c>
@@ -1465,11 +1527,14 @@
       <c r="J20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="K20" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
@@ -1501,10 +1566,13 @@
         <v>96</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -1536,10 +1604,13 @@
         <v>96</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -1571,10 +1642,13 @@
         <v>96</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -1606,10 +1680,13 @@
         <v>96</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
@@ -1641,9 +1718,11 @@
         <v>96</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N25" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -1652,8 +1731,9 @@
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -1684,11 +1764,14 @@
       <c r="J26" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22">
+      <c r="K26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1719,11 +1802,14 @@
       <c r="J27" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22">
+      <c r="K27" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -1754,11 +1840,14 @@
       <c r="J28" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="K28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -1789,11 +1878,14 @@
       <c r="J29" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
+      <c r="K29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1824,11 +1916,14 @@
       <c r="J30" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="K30" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1859,11 +1954,14 @@
       <c r="J31" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
+      <c r="K31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1894,11 +1992,14 @@
       <c r="J32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
+      <c r="K32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -1929,11 +2030,14 @@
       <c r="J33" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
+      <c r="K33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>90</v>
       </c>
@@ -1964,11 +2068,14 @@
       <c r="J34" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
+      <c r="K34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1999,11 +2106,14 @@
       <c r="J35" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
+      <c r="K35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -2034,11 +2144,14 @@
       <c r="J36" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
+      <c r="K36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -2069,11 +2182,14 @@
       <c r="J37" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22">
+      <c r="K37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -2104,11 +2220,14 @@
       <c r="J38" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
+      <c r="K38" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -2139,11 +2258,14 @@
       <c r="J39" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
+      <c r="K39" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>91</v>
       </c>
@@ -2174,10 +2296,12 @@
       <c r="J40" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N40" s="3"/>
+      <c r="K40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
@@ -2186,8 +2310,9 @@
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
-    </row>
-    <row r="41" spans="1:22">
+      <c r="W40" s="3"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>57</v>
       </c>
@@ -2218,12 +2343,14 @@
       <c r="J41" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L41" s="2"/>
+      <c r="K41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M41" s="2"/>
-      <c r="N41" s="3"/>
+      <c r="N41" s="2"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
@@ -2232,8 +2359,9 @@
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
-    </row>
-    <row r="42" spans="1:22">
+      <c r="W41" s="3"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
@@ -2264,11 +2392,14 @@
       <c r="J42" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
+      <c r="K42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -2299,11 +2430,14 @@
       <c r="J43" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
+      <c r="K43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -2334,11 +2468,14 @@
       <c r="J44" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
+      <c r="K44" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2369,10 +2506,12 @@
       <c r="J45" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N45" s="3"/>
+      <c r="K45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
@@ -2381,8 +2520,9 @@
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
-    </row>
-    <row r="46" spans="1:22">
+      <c r="W45" s="3"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -2413,11 +2553,14 @@
       <c r="J46" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K46" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22">
+      <c r="K46" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>60</v>
       </c>
@@ -2448,11 +2591,14 @@
       <c r="J47" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22">
+      <c r="K47" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -2483,10 +2629,12 @@
       <c r="J48" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N48" s="3"/>
+      <c r="K48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
@@ -2495,8 +2643,9 @@
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
-    </row>
-    <row r="49" spans="1:22">
+      <c r="W48" s="3"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>36</v>
       </c>
@@ -2527,11 +2676,14 @@
       <c r="J49" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22">
+      <c r="K49" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>61</v>
       </c>
@@ -2562,11 +2714,14 @@
       <c r="J50" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22">
+      <c r="K50" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
@@ -2597,11 +2752,14 @@
       <c r="J51" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22">
+      <c r="K51" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -2632,11 +2790,14 @@
       <c r="J52" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22">
+      <c r="K52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -2667,10 +2828,12 @@
       <c r="J53" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N53" s="3"/>
+      <c r="K53" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
@@ -2679,8 +2842,9 @@
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
-    </row>
-    <row r="54" spans="1:22">
+      <c r="W53" s="3"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -2711,11 +2875,14 @@
       <c r="J54" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22">
+      <c r="K54" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -2747,10 +2914,13 @@
         <v>96</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
@@ -2782,10 +2952,13 @@
         <v>96</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
@@ -2817,10 +2990,13 @@
         <v>96</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>21</v>
       </c>
@@ -2852,11 +3028,13 @@
         <v>96</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L58" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M58" s="2"/>
-      <c r="N58" s="3"/>
+      <c r="N58" s="2"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
@@ -2865,8 +3043,9 @@
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
       <c r="V58" s="3"/>
-    </row>
-    <row r="59" spans="1:22">
+      <c r="W58" s="3"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>34</v>
       </c>
@@ -2898,11 +3077,13 @@
         <v>96</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L59" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M59" s="2"/>
-      <c r="N59" s="3"/>
+      <c r="N59" s="2"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
@@ -2911,8 +3092,9 @@
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
       <c r="V59" s="3"/>
-    </row>
-    <row r="60" spans="1:22">
+      <c r="W59" s="3"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -2944,11 +3126,13 @@
         <v>96</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L60" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="M60" s="2"/>
-      <c r="N60" s="3"/>
+      <c r="N60" s="2"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
@@ -2957,8 +3141,9 @@
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="3"/>
-    </row>
-    <row r="61" spans="1:22">
+      <c r="W60" s="3"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>19</v>
       </c>
@@ -2990,10 +3175,13 @@
         <v>96</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>22</v>
       </c>
@@ -3025,10 +3213,13 @@
         <v>96</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="63" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -3060,10 +3251,13 @@
         <v>96</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
@@ -3095,10 +3289,13 @@
         <v>96</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>32</v>
       </c>
@@ -3130,10 +3327,13 @@
         <v>96</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>27</v>
       </c>
@@ -3165,10 +3365,13 @@
         <v>96</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>14</v>
       </c>
@@ -3200,9 +3403,11 @@
         <v>96</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N67" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
@@ -3211,8 +3416,9 @@
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
       <c r="V67" s="3"/>
-    </row>
-    <row r="68" spans="1:22">
+      <c r="W67" s="3"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>23</v>
       </c>
@@ -3244,10 +3450,13 @@
         <v>96</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>13</v>
       </c>
@@ -3279,10 +3488,13 @@
         <v>96</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="70" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>20</v>
       </c>
@@ -3314,10 +3526,13 @@
         <v>96</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>26</v>
       </c>
@@ -3349,10 +3564,13 @@
         <v>96</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>18</v>
       </c>
@@ -3384,10 +3602,13 @@
         <v>96</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>16</v>
       </c>
@@ -3419,9 +3640,11 @@
         <v>96</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N73" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
@@ -3430,8 +3653,9 @@
       <c r="T73" s="3"/>
       <c r="U73" s="3"/>
       <c r="V73" s="3"/>
-    </row>
-    <row r="74" spans="1:22">
+      <c r="W73" s="3"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>31</v>
       </c>
@@ -3463,10 +3687,13 @@
         <v>96</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>33</v>
       </c>
@@ -3498,10 +3725,13 @@
         <v>96</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="76" spans="1:22">
+        <v>96</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
@@ -3532,11 +3762,14 @@
       <c r="J76" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K76" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22">
+      <c r="K76" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
@@ -3567,11 +3800,14 @@
       <c r="J77" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K77" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22">
+      <c r="K77" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>37</v>
       </c>
@@ -3602,10 +3838,12 @@
       <c r="J78" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K78" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N78" s="3"/>
+      <c r="K78" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
@@ -3614,8 +3852,9 @@
       <c r="T78" s="3"/>
       <c r="U78" s="3"/>
       <c r="V78" s="3"/>
-    </row>
-    <row r="79" spans="1:22">
+      <c r="W78" s="3"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>68</v>
       </c>
@@ -3646,11 +3885,14 @@
       <c r="J79" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K79" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="1:22">
+      <c r="K79" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>69</v>
       </c>
@@ -3681,11 +3923,14 @@
       <c r="J80" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K80" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22">
+      <c r="K80" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -3716,10 +3961,12 @@
       <c r="J81" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K81" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="N81" s="3"/>
+      <c r="K81" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
@@ -3728,6 +3975,7 @@
       <c r="T81" s="3"/>
       <c r="U81" s="3"/>
       <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:V81">
@@ -3739,24 +3987,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>